<commit_message>
All in Working Condition
</commit_message>
<xml_diff>
--- a/WIP/files/Q04.xlsx
+++ b/WIP/files/Q04.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Steffin Rayen\Desktop\GIT_WORKSPACE\fluffy-chainsaw\WIP\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7A210B3-E7C1-405D-BA3A-25C2B4C5FAC8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6032FB77-A55B-4981-BE38-0D13BCEC4105}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="7848" xr2:uid="{AE9B49F7-EE13-4D7D-9259-C3D9EC769723}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9576" windowHeight="7848" xr2:uid="{FDD0F107-B62F-4A7E-927E-CCC3F4EFB9B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Details" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
   <si>
     <t>Account Number</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>Customer ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> XXXXXXX</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ABC</t>
   </si>
 </sst>
 </file>
@@ -384,12 +390,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B372E14-6334-4094-88C8-85818E2412B5}">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D63F1DA1-6939-4F46-9C4C-5CF1DC6BEFBD}">
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -404,6 +408,50 @@
         <v>2</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>324234234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>324234234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>324234234</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>324234234</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>